<commit_message>
commented stuff out, made stuff work
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Pivot Table" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Pivot Table" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data'!$A$1:$X$9</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cacheId="1" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -25,21 +27,33 @@
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="165" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
-      <family val="2"/>
-      <b val="1"/>
+      <family val="0"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
+      <b val="1"/>
       <sz val="10"/>
     </font>
   </fonts>
@@ -60,265 +74,286 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="medium"/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right/>
+      <top style="medium"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="medium"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
+      <right style="medium"/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <left style="medium"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
+      <left style="thin"/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <right style="medium"/>
+      <top style="thin"/>
+      <bottom style="medium"/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  <cellStyleXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="46">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="22">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="22">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="24">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="2"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="4">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="3"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="5">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="6"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" pivotButton="0" quotePrefix="0" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="6"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="22">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="21">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="22">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="20">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="25">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="24">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="23">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pivot Table Field" xfId="1"/>
-    <cellStyle name="Pivot Table Corner" xfId="2"/>
-    <cellStyle name="Pivot Table Value" xfId="3"/>
-    <cellStyle name="Pivot Table Category" xfId="4"/>
-    <cellStyle name="Pivot Table Title" xfId="5"/>
-    <cellStyle name="Pivot Table Result" xfId="6"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle name="Pivot Table Category" xfId="6"/>
+    <cellStyle name="Pivot Table Corner" xfId="7"/>
+    <cellStyle name="Pivot Table Field" xfId="8"/>
+    <cellStyle name="Pivot Table Result" xfId="9"/>
+    <cellStyle name="Pivot Table Title" xfId="10"/>
+    <cellStyle name="Pivot Table Value" xfId="11"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -391,7 +426,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" refreshedDate="0" createdVersion="3" recordCount="8" r:id="rId1">
+<pivotCacheDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" createdVersion="3" recordCount="8" r:id="rId1">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:X9" sheet="Data"/>
   </cacheSource>
@@ -808,7 +843,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="0" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="0" minRefreshableVersion="0" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="1" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="0" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" r:id="rId1">
+<pivotTableDefinition xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DataPilot1" cacheId="1" dataOnRows="0" dataCaption="Values" showError="0" showMissing="1" updatedVersion="0" minRefreshableVersion="0" asteriskTotals="0" showItems="1" editData="0" disableFieldList="0" showCalcMbrs="1" visualTotals="1" showMultipleLabel="1" showDataDropDown="1" showDrill="1" printDrill="0" showMemberPropertyTips="1" showDataTips="1" enableWizard="1" enableDrill="1" enableFieldProperties="1" preserveFormatting="1" useAutoFormatting="0" pageWrap="0" pageOverThenDown="0" subtotalHiddenItems="0" rowGrandTotals="1" colGrandTotals="1" fieldPrintTitles="0" itemPrintTitles="1" mergeItem="0" showDropZones="1" createdVersion="0" indent="0" showEmptyRow="0" showEmptyCol="0" showHeaders="1" compact="0" outline="0" outlineData="0" compactData="0" published="0" gridDropZones="0" immersive="1" multipleFieldFilters="0" chartFormat="0" fieldListSortAscending="0" mdxSubqueries="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" r:id="rId1">
   <location ref="A1:J4" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="24">
     <pivotField showDropDowns="1" compact="0" outline="1" subtotalTop="1" dragToRow="1" dragToCol="1" dragToPage="1" dragToData="1" dragOff="1" showAll="0" topAutoShow="1" itemPageCount="10" sortType="manual" defaultSubtotal="1"/>
@@ -850,18 +885,49 @@
     <field x="-2"/>
   </colFields>
   <dataFields count="9">
-    <dataField name="Average - U-A[In]" fld="2" subtotal="average" showDataAs="normal" baseField="0" baseItem="0"/>
-    <dataField name="Average - U-A[%]" fld="4" subtotal="average" showDataAs="normal" baseField="0" baseItem="0" numFmtId="2"/>
-    <dataField name="Average - L-A[In]" fld="5" subtotal="average" showDataAs="normal" baseField="0" baseItem="0"/>
-    <dataField name="Average - L-A[%]" fld="7" subtotal="average" showDataAs="normal" baseField="0" baseItem="0" numFmtId="2"/>
-    <dataField name="Average - U-T[In]" fld="13" subtotal="average" showDataAs="normal" baseField="0" baseItem="0"/>
-    <dataField name="Average - U-T[%]" fld="15" subtotal="average" showDataAs="normal" baseField="0" baseItem="0" numFmtId="2"/>
-    <dataField name="Average - L-T[In]" fld="16" subtotal="average" showDataAs="normal" baseField="0" baseItem="0"/>
-    <dataField name="Average - L-T[%]" fld="18" subtotal="average" showDataAs="normal" baseField="0" baseItem="0" numFmtId="2"/>
-    <dataField name="Average - Total Pts" fld="23" subtotal="average" showDataAs="normal" baseField="0" baseItem="0"/>
+    <dataField name="Average - U-A[In]" fld="2" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="164"/>
+    <dataField name="Average - U-A[%]" fld="4" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="165"/>
+    <dataField name="Average - L-A[In]" fld="5" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="164"/>
+    <dataField name="Average - L-A[%]" fld="7" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="165"/>
+    <dataField name="Average - U-T[In]" fld="13" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="164"/>
+    <dataField name="Average - U-T[%]" fld="15" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="165"/>
+    <dataField name="Average - L-T[In]" fld="16" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="164"/>
+    <dataField name="Average - L-T[%]" fld="18" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="165"/>
+    <dataField name="Average - Total Pts" fld="23" subtotal="average" showDataAs="normal" baseField="-1" baseItem="1048832" numFmtId="164"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Data" displayName="Data" ref="A1:X50" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <tableColumns count="24">
+    <tableColumn id="1" name="Match #"/>
+    <tableColumn id="2" name="Team #"/>
+    <tableColumn id="3" name="U-A[In]"/>
+    <tableColumn id="4" name="U-A[Tot]"/>
+    <tableColumn id="5" name="U-A[%]"/>
+    <tableColumn id="6" name="L-A[In]"/>
+    <tableColumn id="7" name="L-A[Tot]"/>
+    <tableColumn id="8" name="L-A[%]"/>
+    <tableColumn id="9" name="TMC"/>
+    <tableColumn id="10" name="Ground"/>
+    <tableColumn id="11" name="Ground Raw"/>
+    <tableColumn id="12" name="HP"/>
+    <tableColumn id="13" name="HP Raw"/>
+    <tableColumn id="14" name="U-T[In]"/>
+    <tableColumn id="15" name="U-T[Tot]"/>
+    <tableColumn id="16" name="U-T[%]"/>
+    <tableColumn id="17" name="L-T[In]"/>
+    <tableColumn id="18" name="L-T[Tot]"/>
+    <tableColumn id="19" name="L-T[%]"/>
+    <tableColumn id="20" name="Climb"/>
+    <tableColumn id="21" name="Cl Pts"/>
+    <tableColumn id="22" name="Cl Time"/>
+    <tableColumn id="23" name="Comments"/>
+    <tableColumn id="24" name="Total Pts"/>
+  </tableColumns>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -875,44 +941,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -939,32 +1005,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -991,24 +1039,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1020,1066 +1050,1375 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="200" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="K1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q11" activeCellId="0" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="0" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col width="8.1640625" customWidth="1" style="4" min="1" max="1"/>
-    <col width="7.5" customWidth="1" style="4" min="2" max="2"/>
-    <col width="9.83203125" customWidth="1" style="4" min="3" max="4"/>
-    <col width="10.1640625" customWidth="1" style="4" min="5" max="5"/>
-    <col width="9.5" customWidth="1" style="4" min="6" max="6"/>
-    <col width="9.83203125" customWidth="1" style="4" min="8" max="8"/>
-    <col width="7.5" customWidth="1" style="4" min="9" max="9"/>
-    <col width="10.1640625" customWidth="1" style="4" min="10" max="10"/>
-    <col width="6.83203125" customWidth="1" style="4" min="12" max="12"/>
-    <col width="10.6640625" customWidth="1" style="4" min="13" max="13"/>
-    <col width="9.6640625" customWidth="1" style="4" min="14" max="15"/>
-    <col width="10" customWidth="1" style="4" min="16" max="16"/>
-    <col width="9.33203125" customWidth="1" style="4" min="17" max="18"/>
-    <col width="9.83203125" customWidth="1" style="4" min="19" max="19"/>
-    <col width="6.1640625" customWidth="1" style="4" min="20" max="20"/>
-    <col width="10.33203125" customWidth="1" style="4" min="21" max="23"/>
+    <col width="8.16" customWidth="1" style="23" min="1" max="1"/>
+    <col width="7.49" customWidth="1" style="23" min="2" max="2"/>
+    <col width="9.83" customWidth="1" style="23" min="3" max="4"/>
+    <col width="10.16" customWidth="1" style="23" min="5" max="5"/>
+    <col width="9.51" customWidth="1" style="23" min="6" max="6"/>
+    <col width="9.83" customWidth="1" style="23" min="8" max="8"/>
+    <col width="7.49" customWidth="1" style="23" min="9" max="9"/>
+    <col width="10.16" customWidth="1" style="23" min="10" max="10"/>
+    <col width="6.83" customWidth="1" style="23" min="12" max="12"/>
+    <col width="10.66" customWidth="1" style="23" min="13" max="13"/>
+    <col width="9.66" customWidth="1" style="23" min="14" max="15"/>
+    <col width="10" customWidth="1" style="23" min="16" max="16"/>
+    <col width="9.33" customWidth="1" style="23" min="17" max="18"/>
+    <col width="9.83" customWidth="1" style="23" min="19" max="19"/>
+    <col width="6.16" customWidth="1" style="23" min="20" max="20"/>
+    <col width="10.33" customWidth="1" style="23" min="21" max="23"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="13" customHeight="1" s="24">
+      <c r="A1" s="23" t="inlineStr">
         <is>
           <t>Match #</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="23" t="inlineStr">
         <is>
           <t>Team #</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="23" t="inlineStr">
         <is>
           <t>U-A[In]</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="23" t="inlineStr">
         <is>
           <t>U-A[Tot]</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="23" t="inlineStr">
         <is>
           <t>U-A[%]</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="23" t="inlineStr">
         <is>
           <t>L-A[In]</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="23" t="inlineStr">
         <is>
           <t>L-A[Tot]</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="23" t="inlineStr">
         <is>
           <t>L-A[%]</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="23" t="inlineStr">
         <is>
           <t>TMC</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="23" t="inlineStr">
         <is>
           <t>Ground</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="23" t="inlineStr">
         <is>
           <t>Ground Raw</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="23" t="inlineStr">
         <is>
           <t>HP</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="23" t="inlineStr">
         <is>
           <t>HP Raw</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="N1" s="23" t="inlineStr">
         <is>
           <t>U-T[In]</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="O1" s="23" t="inlineStr">
         <is>
           <t>U-T[Tot]</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="P1" s="23" t="inlineStr">
         <is>
           <t>U-T[%]</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="Q1" s="23" t="inlineStr">
         <is>
           <t>L-T[In]</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="R1" s="23" t="inlineStr">
         <is>
           <t>L-T[Tot]</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
+      <c r="S1" s="23" t="inlineStr">
         <is>
           <t>L-T[%]</t>
         </is>
       </c>
-      <c r="T1" t="inlineStr">
+      <c r="T1" s="23" t="inlineStr">
         <is>
           <t>Climb</t>
         </is>
       </c>
-      <c r="U1" t="inlineStr">
+      <c r="U1" s="23" t="inlineStr">
         <is>
           <t>Cl Pts</t>
         </is>
       </c>
-      <c r="V1" t="inlineStr">
+      <c r="V1" s="23" t="inlineStr">
         <is>
           <t>Cl Time</t>
         </is>
       </c>
-      <c r="W1" t="inlineStr">
+      <c r="W1" s="23" t="inlineStr">
         <is>
           <t>Comments</t>
         </is>
       </c>
-      <c r="X1" t="inlineStr">
+      <c r="X1" s="23" t="inlineStr">
         <is>
           <t>Total Pts</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" ht="13" customHeight="1" s="24">
+      <c r="A2" s="23" t="n">
         <v>64</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="23" t="n">
         <v>2851</v>
       </c>
-      <c r="C2" t="n">
-        <v>4</v>
-      </c>
-      <c r="D2" t="n">
+      <c r="C2" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="25">
         <f>C2/D2</f>
         <v/>
       </c>
-      <c r="F2" t="n">
-        <v>4</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="F2" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="25">
         <f>F2/G2</f>
         <v/>
       </c>
-      <c r="I2" t="n">
-        <v>4</v>
-      </c>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="I2" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J2" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K2">
+      <c r="K2" s="23">
         <f>IF(J2="Yes", 1, IF(J2="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L2" s="3" t="inlineStr">
+      <c r="L2" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M2">
+      <c r="M2" s="23">
         <f>IF(L2="Yes", 1, IF(L2="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N2" t="n">
+      <c r="N2" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="25">
         <f>N2/O2</f>
         <v/>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="25">
         <f>Q2/R2</f>
         <v/>
       </c>
-      <c r="T2" t="inlineStr">
+      <c r="T2" s="23" t="inlineStr">
         <is>
           <t>TRAV</t>
         </is>
       </c>
-      <c r="U2">
+      <c r="U2" s="23">
         <f>IF(T2="TRAV", 15, IF(T2="HIGH", 10, IF(T2="MID", 6, IF(T2="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V2" s="5" t="n"/>
-      <c r="W2" t="inlineStr">
+      <c r="V2" s="27" t="n"/>
+      <c r="W2" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X2">
+      <c r="X2" s="23">
         <f>(C2*4)+(F2*2)+(N2*2)+(Q2*1)+(U2)</f>
         <v/>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" ht="13" customHeight="1" s="24">
+      <c r="A3" s="23" t="n">
         <v>32</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="23" t="n">
         <v>217</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="25">
         <f>C3/D3</f>
         <v/>
       </c>
-      <c r="F3" t="n">
-        <v>4</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="F3" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="25">
         <f>F3/G3</f>
         <v/>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="J3" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K3">
+      <c r="K3" s="23">
         <f>IF(J3="Yes", 1, IF(J3="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L3" s="3" t="inlineStr">
+      <c r="L3" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="M3">
+      <c r="M3" s="23">
         <f>IF(L3="Yes", 1, IF(L3="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N3" t="n">
+      <c r="N3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O3" t="n">
+      <c r="O3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="25">
         <f>N3/O3</f>
         <v/>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R3" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="S3" s="2">
+      <c r="S3" s="25">
         <f>Q3/R3</f>
         <v/>
       </c>
-      <c r="T3" t="inlineStr">
+      <c r="T3" s="23" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="U3">
+      <c r="U3" s="23">
         <f>IF(T3="TRAV", 15, IF(T3="HIGH", 10, IF(T3="MID", 6, IF(T3="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V3" s="5" t="n"/>
-      <c r="W3" t="inlineStr">
+      <c r="V3" s="27" t="n"/>
+      <c r="W3" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X3">
+      <c r="X3" s="23">
         <f>(C3*4)+(F3*2)+(N3*2)+(Q3*1)+(U3)</f>
         <v/>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="n">
+    <row r="4" ht="13" customHeight="1" s="24">
+      <c r="A4" s="23" t="n">
         <v>64</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="23" t="n">
         <v>217</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C4" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D4" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="25">
         <f>C4/D4</f>
         <v/>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="23" t="n">
         <v>8</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="25">
         <f>F4/G4</f>
         <v/>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="J4" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K4">
+      <c r="K4" s="23">
         <f>IF(J4="Yes", 1, IF(J4="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L4" s="3" t="inlineStr">
+      <c r="L4" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M4">
+      <c r="M4" s="23">
         <f>IF(L4="Yes", 1, IF(L4="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N4" t="n">
+      <c r="N4" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O4" t="n">
+      <c r="O4" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="25">
         <f>N4/O4</f>
         <v/>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="S4" s="2">
+      <c r="S4" s="25">
         <f>Q4/R4</f>
         <v/>
       </c>
-      <c r="T4" t="inlineStr">
+      <c r="T4" s="23" t="inlineStr">
         <is>
           <t>MID</t>
         </is>
       </c>
-      <c r="U4">
+      <c r="U4" s="23">
         <f>IF(T4="TRAV", 15, IF(T4="HIGH", 10, IF(T4="MID", 6, IF(T4="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V4" s="5" t="n"/>
-      <c r="W4" t="inlineStr">
+      <c r="V4" s="27" t="n"/>
+      <c r="W4" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X4">
+      <c r="X4" s="23">
         <f>(C4*4)+(F4*2)+(N4*2)+(Q4*1)+(U4)</f>
         <v/>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
+    <row r="5" ht="13" customHeight="1" s="24">
+      <c r="A5" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="n">
         <v>2851</v>
       </c>
-      <c r="C5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="C5" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="25">
         <f>C5/D5</f>
         <v/>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="23" t="n">
         <v>9</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="25">
         <f>F5/G5</f>
         <v/>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="J5" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="K5">
+      <c r="K5" s="23">
         <f>IF(J5="Yes", 1, IF(J5="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L5" s="3" t="inlineStr">
+      <c r="L5" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M5">
+      <c r="M5" s="23">
         <f>IF(L5="Yes", 1, IF(L5="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N5" t="n">
-        <v>4</v>
-      </c>
-      <c r="O5" t="n">
+      <c r="N5" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="O5" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="25">
         <f>N5/O5</f>
         <v/>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="25">
         <f>Q5/R5</f>
         <v/>
       </c>
-      <c r="T5" t="inlineStr">
+      <c r="T5" s="23" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
       </c>
-      <c r="U5">
+      <c r="U5" s="23">
         <f>IF(T5="TRAV", 15, IF(T5="HIGH", 10, IF(T5="MID", 6, IF(T5="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V5" s="5" t="n"/>
-      <c r="W5" t="inlineStr">
+      <c r="V5" s="27" t="n"/>
+      <c r="W5" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X5">
+      <c r="X5" s="23">
         <f>(C5*4)+(F5*2)+(N5*2)+(Q5*1)+(U5)</f>
         <v/>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="n">
+    <row r="6" ht="13" customHeight="1" s="24">
+      <c r="A6" s="23" t="n">
         <v>34</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="23" t="n">
         <v>1718</v>
       </c>
-      <c r="C6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="25">
         <f>C6/D6</f>
         <v/>
       </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="n">
+      <c r="F6" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="25">
         <f>F6/G6</f>
         <v/>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="J6" s="3" t="inlineStr">
+      <c r="J6" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K6">
+      <c r="K6" s="23">
         <f>IF(J6="Yes", 1, IF(J6="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L6" s="3" t="inlineStr">
+      <c r="L6" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M6">
+      <c r="M6" s="23">
         <f>IF(L6="Yes", 1, IF(L6="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N6" t="n">
+      <c r="N6" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="O6" t="n">
+      <c r="O6" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="25">
         <f>N6/O6</f>
         <v/>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" s="23" t="n">
         <v>10</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6" s="25">
         <f>Q6/R6</f>
         <v/>
       </c>
-      <c r="T6" t="inlineStr">
+      <c r="T6" s="23" t="inlineStr">
         <is>
           <t>TRAV</t>
         </is>
       </c>
-      <c r="U6">
+      <c r="U6" s="23">
         <f>IF(T6="TRAV", 15, IF(T6="HIGH", 10, IF(T6="MID", 6, IF(T6="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V6" s="5" t="n"/>
-      <c r="W6" t="inlineStr">
+      <c r="V6" s="27" t="n"/>
+      <c r="W6" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X6">
+      <c r="X6" s="23">
         <f>(C6*4)+(F6*2)+(N6*2)+(Q6*1)+(U6)</f>
         <v/>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="n">
+    <row r="7" ht="13" customHeight="1" s="24">
+      <c r="A7" s="23" t="n">
         <v>56</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="23" t="n">
         <v>1718</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C7" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="25">
         <f>C7/D7</f>
         <v/>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="25">
         <f>F7/G7</f>
         <v/>
       </c>
-      <c r="I7" t="n">
-        <v>4</v>
-      </c>
-      <c r="J7" s="3" t="inlineStr">
+      <c r="I7" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K7">
+      <c r="K7" s="23">
         <f>IF(J7="Yes", 1, IF(J7="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L7" s="3" t="inlineStr">
+      <c r="L7" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="M7">
+      <c r="M7" s="23">
         <f>IF(L7="Yes", 1, IF(L7="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N7" t="n">
+      <c r="N7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O7" t="n">
+      <c r="O7" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="25">
         <f>N7/O7</f>
         <v/>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="S7" s="2">
+      <c r="S7" s="25">
         <f>Q7/R7</f>
         <v/>
       </c>
-      <c r="T7" t="inlineStr">
+      <c r="T7" s="23" t="inlineStr">
         <is>
           <t>HIGH</t>
         </is>
       </c>
-      <c r="U7">
+      <c r="U7" s="23">
         <f>IF(T7="TRAV", 15, IF(T7="HIGH", 10, IF(T7="MID", 6, IF(T7="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V7" s="5" t="n"/>
-      <c r="W7" t="inlineStr">
+      <c r="V7" s="27" t="n"/>
+      <c r="W7" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X7">
+      <c r="X7" s="23">
         <f>(C7*4)+(F7*2)+(N7*2)+(Q7*1)+(U7)</f>
         <v/>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="n">
+    <row r="8" ht="13" customHeight="1" s="24">
+      <c r="A8" s="23" t="n">
         <v>86</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="23" t="n">
         <v>2834</v>
       </c>
-      <c r="C8" t="n">
+      <c r="C8" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="D8" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="E8" s="25">
         <f>C8/D8</f>
         <v/>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="G8" t="n">
-        <v>4</v>
-      </c>
-      <c r="H8" s="2">
+      <c r="G8" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="H8" s="25">
         <f>F8/G8</f>
         <v/>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="J8" s="3" t="inlineStr">
+      <c r="J8" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K8">
+      <c r="K8" s="23">
         <f>IF(J8="Yes", 1, IF(J8="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L8" s="3" t="inlineStr">
+      <c r="L8" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M8">
+      <c r="M8" s="23">
         <f>IF(L8="Yes", 1, IF(L8="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N8" t="n">
+      <c r="N8" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="O8" t="n">
+      <c r="O8" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="25">
         <f>N8/O8</f>
         <v/>
       </c>
-      <c r="Q8" t="n">
-        <v>4</v>
-      </c>
-      <c r="R8" t="n">
+      <c r="Q8" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="R8" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="S8" s="2">
+      <c r="S8" s="25">
         <f>Q8/R8</f>
         <v/>
       </c>
-      <c r="T8" t="inlineStr">
+      <c r="T8" s="23" t="inlineStr">
         <is>
           <t>MID</t>
         </is>
       </c>
-      <c r="U8">
+      <c r="U8" s="23">
         <f>IF(T8="TRAV", 15, IF(T8="HIGH", 10, IF(T8="MID", 6, IF(T8="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V8" s="5" t="n"/>
-      <c r="W8" t="inlineStr">
+      <c r="V8" s="27" t="n"/>
+      <c r="W8" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X8">
+      <c r="X8" s="23">
         <f>(C8*4)+(F8*2)+(N8*2)+(Q8*1)+(U8)</f>
         <v/>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="n">
+    <row r="9" ht="13" customHeight="1" s="24">
+      <c r="A9" s="23" t="n">
         <v>23</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="23" t="n">
         <v>217</v>
       </c>
-      <c r="C9" t="n">
-        <v>4</v>
-      </c>
-      <c r="D9" t="n">
+      <c r="C9" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="23" t="n">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="25">
         <f>C9/D9</f>
         <v/>
       </c>
-      <c r="F9" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" t="n">
+      <c r="F9" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="25">
         <f>F9/G9</f>
         <v/>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="J9" s="3" t="inlineStr">
+      <c r="J9" s="26" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="K9">
+      <c r="K9" s="23">
         <f>IF(J9="Yes", 1, IF(J9="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="L9" s="3" t="inlineStr">
+      <c r="L9" s="26" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="M9">
+      <c r="M9" s="23">
         <f>IF(L9="Yes", 1, IF(L9="No",0,"na"))</f>
         <v/>
       </c>
-      <c r="N9" t="n">
+      <c r="N9" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O9" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="25">
         <f>N9/O9</f>
         <v/>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="S9" s="2">
+      <c r="S9" s="25">
         <f>Q9/R9</f>
         <v/>
       </c>
-      <c r="T9" t="inlineStr">
+      <c r="T9" s="23" t="inlineStr">
         <is>
           <t>LOW</t>
         </is>
       </c>
-      <c r="U9">
+      <c r="U9" s="23">
         <f>IF(T9="TRAV", 15, IF(T9="HIGH", 10, IF(T9="MID", 6, IF(T9="LOW", 4, "na"))))</f>
         <v/>
       </c>
-      <c r="V9" s="5" t="n"/>
-      <c r="W9" t="inlineStr">
+      <c r="V9" s="27" t="n"/>
+      <c r="W9" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf</t>
         </is>
       </c>
-      <c r="X9">
+      <c r="X9" s="23">
         <f>(C9*4)+(F9*2)+(N9*2)+(Q9*1)+(U9)</f>
         <v/>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="n">
+    <row r="10" ht="13" customHeight="1" s="24">
+      <c r="A10" s="23" t="n">
         <v>64</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="23" t="n">
         <v>2851</v>
       </c>
-      <c r="C10" t="n">
-        <v>4</v>
-      </c>
-      <c r="D10" t="n">
+      <c r="C10" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="F10" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" t="n">
+      <c r="F10" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="I10" t="n">
-        <v>4</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="I10" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="J10" s="23" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L10" s="23" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="N10" t="n">
+      <c r="N10" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O10" s="23" t="n">
         <v>5</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="T10" t="inlineStr">
+      <c r="T10" s="23" t="inlineStr">
         <is>
           <t>TRAV</t>
         </is>
       </c>
-      <c r="V10" t="n">
+      <c r="V10" s="23" t="n">
         <v>15</v>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="W10" s="23" t="inlineStr">
         <is>
           <t>fmdkmfdlaf, I dunno</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>64</v>
+      </c>
+      <c r="B11" t="n">
+        <v>2851</v>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" t="n">
+        <v>6</v>
+      </c>
+      <c r="I11" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N11" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" t="n">
+        <v>6</v>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>TRAV</t>
+        </is>
+      </c>
+      <c r="V11" t="n">
+        <v>15</v>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fmdkmfdlaf, I dunno
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>64</v>
+      </c>
+      <c r="B12" t="n">
+        <v>2851</v>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" t="n">
+        <v>4</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="I12" t="n">
+        <v>4</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="N12" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" t="n">
+        <v>6</v>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>TRAV</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>15</v>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">fmdkmfdlaf, TEST
+</t>
         </is>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:X9"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.515625" defaultRowHeight="13" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="13" customHeight="1" s="24">
+      <c r="A1" s="28" t="n"/>
+      <c r="B1" s="29" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="C1" s="30" t="n"/>
+      <c r="D1" s="30" t="n"/>
+      <c r="E1" s="30" t="n"/>
+      <c r="F1" s="30" t="n"/>
+      <c r="G1" s="30" t="n"/>
+      <c r="H1" s="30" t="n"/>
+      <c r="I1" s="30" t="n"/>
+      <c r="J1" s="31" t="n"/>
+    </row>
+    <row r="2" ht="13" customHeight="1" s="24">
+      <c r="A2" s="32" t="inlineStr">
+        <is>
+          <t>Team #</t>
+        </is>
+      </c>
+      <c r="B2" s="33" t="inlineStr">
+        <is>
+          <t>Average - U-A[In]</t>
+        </is>
+      </c>
+      <c r="C2" s="34" t="inlineStr">
+        <is>
+          <t>Average - U-A[%]</t>
+        </is>
+      </c>
+      <c r="D2" s="34" t="inlineStr">
+        <is>
+          <t>Average - L-A[In]</t>
+        </is>
+      </c>
+      <c r="E2" s="34" t="inlineStr">
+        <is>
+          <t>Average - L-A[%]</t>
+        </is>
+      </c>
+      <c r="F2" s="34" t="inlineStr">
+        <is>
+          <t>Average - U-T[In]</t>
+        </is>
+      </c>
+      <c r="G2" s="34" t="inlineStr">
+        <is>
+          <t>Average - U-T[%]</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="inlineStr">
+        <is>
+          <t>Average - L-T[In]</t>
+        </is>
+      </c>
+      <c r="I2" s="34" t="inlineStr">
+        <is>
+          <t>Average - L-T[%]</t>
+        </is>
+      </c>
+      <c r="J2" s="35" t="inlineStr">
+        <is>
+          <t>Average - Total Pts</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="13" customHeight="1" s="24">
+      <c r="A3" s="36" t="n">
+        <v>2851</v>
+      </c>
+      <c r="B3" s="37" t="n">
+        <v>4</v>
+      </c>
+      <c r="C3" s="38" t="n">
+        <v>0.6857142857142861</v>
+      </c>
+      <c r="D3" s="39" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" s="38" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F3" s="39" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G3" s="38" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H3" s="39" t="n">
+        <v>4</v>
+      </c>
+      <c r="I3" s="38" t="n">
+        <v>1.16666666666667</v>
+      </c>
+      <c r="J3" s="40" t="n">
+        <v>46.5</v>
+      </c>
+    </row>
+    <row r="4" ht="13" customHeight="1" s="24">
+      <c r="A4" s="41" t="inlineStr">
+        <is>
+          <t>Total Result</t>
+        </is>
+      </c>
+      <c r="B4" s="42" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="43" t="n">
+        <v>0.6857142857142861</v>
+      </c>
+      <c r="D4" s="44" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" s="43" t="n">
+        <v>0.666666666666667</v>
+      </c>
+      <c r="F4" s="44" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="G4" s="43" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H4" s="44" t="n">
+        <v>4</v>
+      </c>
+      <c r="I4" s="43" t="n">
+        <v>1.16666666666667</v>
+      </c>
+      <c r="J4" s="45" t="n">
+        <v>46.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
     <evenHeader/>
@@ -2090,160 +2429,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="6" t="n"/>
-      <c r="B1" s="7" t="inlineStr">
-        <is>
-          <t>Data</t>
-        </is>
-      </c>
-      <c r="C1" s="8" t="n"/>
-      <c r="D1" s="8" t="n"/>
-      <c r="E1" s="8" t="n"/>
-      <c r="F1" s="8" t="n"/>
-      <c r="G1" s="8" t="n"/>
-      <c r="H1" s="8" t="n"/>
-      <c r="I1" s="8" t="n"/>
-      <c r="J1" s="9" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="10" t="inlineStr">
-        <is>
-          <t>Team #</t>
-        </is>
-      </c>
-      <c r="B2" s="11" t="inlineStr">
-        <is>
-          <t>Average - U-A[In]</t>
-        </is>
-      </c>
-      <c r="C2" s="12" t="inlineStr">
-        <is>
-          <t>Average - U-A[%]</t>
-        </is>
-      </c>
-      <c r="D2" s="12" t="inlineStr">
-        <is>
-          <t>Average - L-A[In]</t>
-        </is>
-      </c>
-      <c r="E2" s="12" t="inlineStr">
-        <is>
-          <t>Average - L-A[%]</t>
-        </is>
-      </c>
-      <c r="F2" s="12" t="inlineStr">
-        <is>
-          <t>Average - U-T[In]</t>
-        </is>
-      </c>
-      <c r="G2" s="12" t="inlineStr">
-        <is>
-          <t>Average - U-T[%]</t>
-        </is>
-      </c>
-      <c r="H2" s="12" t="inlineStr">
-        <is>
-          <t>Average - L-T[In]</t>
-        </is>
-      </c>
-      <c r="I2" s="12" t="inlineStr">
-        <is>
-          <t>Average - L-T[%]</t>
-        </is>
-      </c>
-      <c r="J2" s="13" t="inlineStr">
-        <is>
-          <t>Average - Total Pts</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="14" t="n">
-        <v>2851</v>
-      </c>
-      <c r="B3" s="15" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" s="16" t="n">
-        <v>0.6857142857142861</v>
-      </c>
-      <c r="D3" s="17" t="n">
-        <v>5</v>
-      </c>
-      <c r="E3" s="16" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F3" s="17" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G3" s="16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="H3" s="17" t="n">
-        <v>4</v>
-      </c>
-      <c r="I3" s="16" t="n">
-        <v>1.16666666666667</v>
-      </c>
-      <c r="J3" s="18" t="n">
-        <v>46.5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="19" t="inlineStr">
-        <is>
-          <t>Total Result</t>
-        </is>
-      </c>
-      <c r="B4" s="20" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" s="21" t="n">
-        <v>0.6857142857142861</v>
-      </c>
-      <c r="D4" s="22" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" s="21" t="n">
-        <v>0.666666666666667</v>
-      </c>
-      <c r="F4" s="22" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="G4" s="21" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="H4" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="I4" s="21" t="n">
-        <v>1.16666666666667</v>
-      </c>
-      <c r="J4" s="23" t="n">
-        <v>46.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentOddEven="0" differentFirst="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>
     <evenFooter/>
     <firstHeader/>

</xml_diff>